<commit_message>
Published state of ETDataset on 15 december 2017
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/industry/industry_flexibility_p2g_electricity.converter.xlsx
+++ b/nodes_source_analyses/industry/industry_flexibility_p2g_electricity.converter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-10340" windowWidth="25600" windowHeight="26800" tabRatio="762" activeTab="1"/>
+    <workbookView xWindow="28800" yWindow="-10340" windowWidth="25600" windowHeight="26800" tabRatio="762" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -747,6 +747,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -754,6 +755,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -761,6 +763,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -768,17 +771,20 @@
       <sz val="16"/>
       <color rgb="FF1F497D"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -786,12 +792,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -814,11 +822,13 @@
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -3015,7 +3025,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3197,8 +3207,8 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3478,8 +3488,8 @@
         <v>51</v>
       </c>
       <c r="E20" s="41">
-        <f>'Research data'!H20</f>
-        <v>80000</v>
+        <f>'Research data'!H19</f>
+        <v>30000</v>
       </c>
       <c r="F20" s="39"/>
       <c r="G20" s="140" t="s">
@@ -3872,7 +3882,7 @@
   <dimension ref="A2:S41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3881,7 +3891,7 @@
     <col min="2" max="2" width="3" style="42" customWidth="1"/>
     <col min="3" max="3" width="34.5" style="42" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="42" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="42" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" style="42" customWidth="1"/>
     <col min="6" max="6" width="10" style="42" customWidth="1"/>
     <col min="7" max="7" width="3" style="42" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" style="42" customWidth="1"/>
@@ -4252,13 +4262,13 @@
       <c r="F19" s="123" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="122" t="e">
+      <c r="H19" s="122">
         <f>J19</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J19" s="157" t="e">
-        <f>Notes!#REF!</f>
-        <v>#REF!</v>
+        <v>30000</v>
+      </c>
+      <c r="J19" s="157">
+        <f>Notes!E50</f>
+        <v>30000</v>
       </c>
       <c r="L19" s="118"/>
       <c r="M19" s="118"/>
@@ -4277,12 +4287,9 @@
       </c>
       <c r="H20" s="158">
         <f>J20</f>
-        <v>80000</v>
-      </c>
-      <c r="J20" s="157">
-        <f>Notes!E36</f>
-        <v>80000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J20" s="157"/>
       <c r="L20" s="118"/>
       <c r="M20" s="118"/>
       <c r="N20" s="118"/>
@@ -4612,7 +4619,7 @@
   <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4924,8 +4931,8 @@
   </sheetPr>
   <dimension ref="A1:O256"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5747,9 +5754,8 @@
     <row r="52" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B52" s="70"/>
       <c r="C52" s="71"/>
-      <c r="E52" s="64" t="e">
-        <f>E51*#REF!</f>
-        <v>#REF!</v>
+      <c r="E52" s="64">
+        <v>0</v>
       </c>
       <c r="F52" s="64" t="s">
         <v>20</v>

</xml_diff>